<commit_message>
Monte Carlo improvements: . FIXES . changed MC solver to ipopt and removed conic relaxation to solve NLP power-flow
</commit_message>
<xml_diff>
--- a/Pyomo/MILP_v1/Input_Files/InputData34_v4.xlsx
+++ b/Pyomo/MILP_v1/Input_Files/InputData34_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Forro\PycharmProjects\MasterThesis\Pyomo\MILP_v1\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F86A97-7733-406D-B417-7363A5789982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7385D1AA-72B5-447B-A62D-62019AD8DB14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="890" activeTab="3" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11325" tabRatio="890" activeTab="5" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
   </bookViews>
   <sheets>
     <sheet name="LineData" sheetId="3" r:id="rId1"/>
@@ -1147,12 +1147,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1642,9 +1642,9 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>24.831999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>13.055999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>13.055999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>13.055999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>2.4319999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>41.696000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>24.831999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>10.335999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>10.335999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>10.335999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2392,9 +2392,9 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2682,9 +2682,9 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>94</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>95</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>96</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>99</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>100</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>102</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>103</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>104</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>105</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>106</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>107</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>108</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>109</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>110</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>111</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>112</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>113</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>114</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>115</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>116</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>117</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>118</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>119</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>120</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>121</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>122</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>123</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>124</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>125</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>126</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>127</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>128</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>129</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>130</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>131</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>132</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>133</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>134</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>135</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>136</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>137</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>138</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>139</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>140</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>141</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>142</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>143</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>144</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>145</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>146</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>147</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>148</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>149</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>150</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>151</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>152</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>153</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>154</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>155</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>156</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>157</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>158</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>159</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>160</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>161</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>162</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>163</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>164</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>165</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>166</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>167</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>168</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>169</v>
       </c>
@@ -4203,15 +4203,15 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4442,7 +4442,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4500,9 +4500,9 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4558,12 +4558,12 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4582,10 +4582,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4593,10 +4593,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4604,10 +4604,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4615,10 +4615,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4626,10 +4626,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4637,10 +4637,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4648,10 +4648,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4659,10 +4659,10 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4670,10 +4670,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4681,10 +4681,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4692,10 +4692,10 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4703,10 +4703,10 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4714,10 +4714,10 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4725,10 +4725,10 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4736,10 +4736,10 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4747,10 +4747,10 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4758,10 +4758,10 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4769,10 +4769,10 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4780,10 +4780,10 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4791,10 +4791,10 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4802,10 +4802,10 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4813,10 +4813,10 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4824,10 +4824,10 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4835,10 +4835,10 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4846,10 +4846,10 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4857,10 +4857,10 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4868,10 +4868,10 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4879,10 +4879,10 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4890,10 +4890,10 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4901,10 +4901,10 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4912,10 +4912,10 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4923,10 +4923,10 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4934,10 +4934,10 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>500000</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -4956,15 +4956,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426FB03F-1F76-4A79-87BD-14907EA3DD39}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4975,14 +4975,91 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>400</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>800</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>27</v>
       </c>
-      <c r="B2">
-        <v>200</v>
-      </c>
-      <c r="C2">
+      <c r="B8">
+        <v>356</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
         <v>0</v>
       </c>
     </row>
@@ -4999,9 +5076,9 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5015,7 +5092,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5029,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5043,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5057,7 +5134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5071,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5085,7 +5162,7 @@
         <v>1.38E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5099,7 +5176,7 @@
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5113,7 +5190,7 @@
         <v>7.1400000000000005E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5127,7 +5204,7 @@
         <v>0.11890000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5141,7 +5218,7 @@
         <v>0.13880000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5155,7 +5232,7 @@
         <v>0.16589999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5169,7 +5246,7 @@
         <v>0.14449999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5183,7 +5260,7 @@
         <v>0.11749999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5197,7 +5274,7 @@
         <v>9.9500000000000005E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5211,7 +5288,7 @@
         <v>7.8799999999999995E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5225,7 +5302,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5239,7 +5316,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5253,7 +5330,7 @@
         <v>2.76E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5267,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5281,7 +5358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5295,7 +5372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5309,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5323,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5337,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5359,15 +5436,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1B3BC8-3C07-47B0-8D22-CF47C6C555E5}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5378,7 +5455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>27</v>
       </c>
@@ -5387,6 +5464,61 @@
       </c>
       <c r="C2">
         <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>150</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5402,9 +5534,9 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5418,7 +5550,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5432,7 +5564,7 @@
         <v>0.79369999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5446,7 +5578,7 @@
         <v>0.80210000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5460,7 +5592,7 @@
         <v>0.85050000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5474,7 +5606,7 @@
         <v>0.81850000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5488,7 +5620,7 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5502,7 +5634,7 @@
         <v>1.0583</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5516,7 +5648,7 @@
         <v>1.1533</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5530,7 +5662,7 @@
         <v>1.1504000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5544,7 +5676,7 @@
         <v>0.95040000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5558,7 +5690,7 @@
         <v>1.1533</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5572,7 +5704,7 @@
         <v>1.0065999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5586,7 +5718,7 @@
         <v>0.86219999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5600,7 +5732,7 @@
         <v>0.37859999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5614,7 +5746,7 @@
         <v>0.45829999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5628,7 +5760,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5642,7 +5774,7 @@
         <v>0.45090000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5656,7 +5788,7 @@
         <v>0.23089999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5670,7 +5802,7 @@
         <v>0.37859999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5684,7 +5816,7 @@
         <v>0.32150000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5698,7 +5830,7 @@
         <v>0.32150000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5712,7 +5844,7 @@
         <v>0.4163</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5726,7 +5858,7 @@
         <v>0.2646</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5740,7 +5872,7 @@
         <v>0.2082</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5765,12 +5897,12 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5787,7 +5919,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -5804,7 +5936,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15</v>
       </c>
@@ -5812,7 +5944,7 @@
         <v>90</v>
       </c>
       <c r="C3">
-        <v>690</v>
+        <v>300</v>
       </c>
       <c r="D3">
         <v>250</v>
@@ -5834,9 +5966,9 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5862,7 +5994,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>34</v>
       </c>
@@ -5888,7 +6020,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>32</v>
       </c>

</xml_diff>